<commit_message>
chore: merged development into webtool
</commit_message>
<xml_diff>
--- a/data/plz_geocoord_matched.xlsx
+++ b/data/plz_geocoord_matched.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Script\districtgenerator\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74F97CD-3ED5-4A13-90FA-C5988F67681A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CAE2A6-5C55-4C7E-99C2-39FBCB1B1351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>PLZ</t>
   </si>
@@ -43,61 +43,34 @@
     <t>01067</t>
   </si>
   <si>
-    <t>TRY2015_42515002705500_Jahr.dat</t>
-  </si>
-  <si>
-    <t>01069</t>
-  </si>
-  <si>
-    <t>TRY2015_42535002703500_Jahr.dat</t>
-  </si>
-  <si>
-    <t>01097</t>
-  </si>
-  <si>
-    <t>TRY2015_42525002706500_Jahr.dat</t>
-  </si>
-  <si>
-    <t>01099</t>
-  </si>
-  <si>
-    <t>TRY2015_42575002708500_Jahr.dat</t>
-  </si>
-  <si>
-    <t>01108</t>
-  </si>
-  <si>
-    <t>TRY2015_42565002714500_Jahr.dat</t>
-  </si>
-  <si>
-    <t>01109</t>
-  </si>
-  <si>
-    <t>TRY2015_42515002711500_Jahr.dat</t>
-  </si>
-  <si>
-    <t>01127</t>
-  </si>
-  <si>
-    <t>TRY2015_42515002707500_Jahr.dat</t>
-  </si>
-  <si>
-    <t>01129</t>
-  </si>
-  <si>
-    <t>TRY2015_42515002709500_Jahr.dat</t>
-  </si>
-  <si>
-    <t>01139</t>
-  </si>
-  <si>
-    <t>TRY2015_42495002706500_Jahr.dat</t>
-  </si>
-  <si>
-    <t>01156</t>
-  </si>
-  <si>
-    <t>TRY2015_42455002707500_Jahr.dat</t>
+    <t>TRY2015_535485100234_Jahr.dat</t>
+  </si>
+  <si>
+    <t>TRY2015_525153133939_Jahr.dat</t>
+  </si>
+  <si>
+    <t>TRY2015_510342136998_Jahr.dat</t>
+  </si>
+  <si>
+    <t>TRY2015_480091078440_Jahr.dat</t>
+  </si>
+  <si>
+    <t>TRY2015_481593115227_Jahr.dat</t>
+  </si>
+  <si>
+    <t>TRY2015_513148094876_Jahr.dat</t>
+  </si>
+  <si>
+    <t>TRY2015_509319069572_Jahr.dat</t>
+  </si>
+  <si>
+    <t>TRY2015_515220074856_Jahr.dat</t>
+  </si>
+  <si>
+    <t>TRY2015_522733105384_Jahr.dat</t>
+  </si>
+  <si>
+    <t>TRY2015_507755060854_Jahr.dat</t>
   </si>
 </sst>
 </file>
@@ -164,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -172,6 +145,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -474,13 +449,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="39" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -503,8 +481,8 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>6</v>
+      <c r="A2" s="4">
+        <v>44137</v>
       </c>
       <c r="B2">
         <v>51.057549599999987</v>
@@ -513,7 +491,7 @@
         <v>13.717064799999999</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E2">
         <v>51.06157970077107</v>
@@ -523,8 +501,8 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>8</v>
+      <c r="A3" s="3">
+        <v>50667</v>
       </c>
       <c r="B3">
         <v>51.039134900000001</v>
@@ -533,7 +511,7 @@
         <v>13.737674800000001</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E3">
         <v>51.042046308508112</v>
@@ -543,8 +521,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>10</v>
+      <c r="A4" s="3">
+        <v>52064</v>
       </c>
       <c r="B4">
         <v>51.065908100000001</v>
@@ -553,7 +531,7 @@
         <v>13.736152499999999</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E4">
         <v>51.070407627228121</v>
@@ -563,8 +541,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>12</v>
+      <c r="A5" s="3">
+        <v>34117</v>
       </c>
       <c r="B5">
         <v>51.087188400000002</v>
@@ -573,7 +551,7 @@
         <v>13.8028038</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5">
         <v>51.086627310398377</v>
@@ -583,8 +561,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>14</v>
+      <c r="A6" s="3">
+        <v>10115</v>
       </c>
       <c r="B6">
         <v>51.144323900000003</v>
@@ -593,7 +571,7 @@
         <v>13.799705700000001</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E6">
         <v>51.142883954834232</v>
@@ -603,8 +581,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>16</v>
+      <c r="A7" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="B7">
         <v>51.1173979</v>
@@ -613,7 +591,7 @@
         <v>13.728314900000001</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E7">
         <v>51.117361114561781</v>
@@ -623,8 +601,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>18</v>
+      <c r="A8" s="3">
+        <v>80331</v>
       </c>
       <c r="B8">
         <v>51.077936600000001</v>
@@ -633,7 +611,7 @@
         <v>13.722437899999999</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E8">
         <v>51.080173609669671</v>
@@ -643,8 +621,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>20</v>
+      <c r="A9" s="3">
+        <v>20354</v>
       </c>
       <c r="B9">
         <v>51.0943744</v>
@@ -653,7 +631,7 @@
         <v>13.7205411</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="E9">
         <v>51.098767414925582</v>
@@ -663,8 +641,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>22</v>
+      <c r="A10" s="3">
+        <v>79100</v>
       </c>
       <c r="B10">
         <v>51.074711899999997</v>
@@ -673,7 +651,7 @@
         <v>13.684631400000001</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E10">
         <v>51.071809179759093</v>
@@ -683,8 +661,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>24</v>
+      <c r="A11" s="3">
+        <v>38100</v>
       </c>
       <c r="B11">
         <v>51.085543999999999</v>
@@ -693,7 +671,7 @@
         <v>13.6276849</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E11">
         <v>51.082949411534422</v>
@@ -702,47 +680,8 @@
         <v>13.629674415765569</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12">
-        <v>51.057549599999987</v>
-      </c>
-      <c r="C12">
-        <v>13.717064799999999</v>
-      </c>
-      <c r="D12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12">
-        <v>51.06157970077107</v>
-      </c>
-      <c r="F12">
-        <v>13.71674948054328</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13">
-        <v>51.039134900000001</v>
-      </c>
-      <c r="C13">
-        <v>13.737674800000001</v>
-      </c>
-      <c r="D13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13">
-        <v>51.042046308508112</v>
-      </c>
-      <c r="F13">
-        <v>13.74475915535144</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change weather data to examples of 10 cities
</commit_message>
<xml_diff>
--- a/data/plz_geocoord_matched.xlsx
+++ b/data/plz_geocoord_matched.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Script\districtgenerator\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74F97CD-3ED5-4A13-90FA-C5988F67681A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EBE6AF8-3107-4006-A186-E36207B9ACE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-5325" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>PLZ</t>
   </si>
@@ -43,61 +43,34 @@
     <t>01067</t>
   </si>
   <si>
-    <t>TRY2015_42515002705500_Jahr.dat</t>
-  </si>
-  <si>
-    <t>01069</t>
-  </si>
-  <si>
-    <t>TRY2015_42535002703500_Jahr.dat</t>
-  </si>
-  <si>
-    <t>01097</t>
-  </si>
-  <si>
-    <t>TRY2015_42525002706500_Jahr.dat</t>
-  </si>
-  <si>
-    <t>01099</t>
-  </si>
-  <si>
-    <t>TRY2015_42575002708500_Jahr.dat</t>
-  </si>
-  <si>
-    <t>01108</t>
-  </si>
-  <si>
-    <t>TRY2015_42565002714500_Jahr.dat</t>
-  </si>
-  <si>
-    <t>01109</t>
-  </si>
-  <si>
-    <t>TRY2015_42515002711500_Jahr.dat</t>
-  </si>
-  <si>
-    <t>01127</t>
-  </si>
-  <si>
-    <t>TRY2015_42515002707500_Jahr.dat</t>
-  </si>
-  <si>
-    <t>01129</t>
-  </si>
-  <si>
-    <t>TRY2015_42515002709500_Jahr.dat</t>
-  </si>
-  <si>
-    <t>01139</t>
-  </si>
-  <si>
-    <t>TRY2015_42495002706500_Jahr.dat</t>
-  </si>
-  <si>
-    <t>01156</t>
-  </si>
-  <si>
-    <t>TRY2015_42455002707500_Jahr.dat</t>
+    <t>TRY2015_535485100234_Jahr.dat</t>
+  </si>
+  <si>
+    <t>TRY2015_525153133939_Jahr.dat</t>
+  </si>
+  <si>
+    <t>TRY2015_510342136998_Jahr.dat</t>
+  </si>
+  <si>
+    <t>TRY2015_480091078440_Jahr.dat</t>
+  </si>
+  <si>
+    <t>TRY2015_481593115227_Jahr.dat</t>
+  </si>
+  <si>
+    <t>TRY2015_513148094876_Jahr.dat</t>
+  </si>
+  <si>
+    <t>TRY2015_509319069572_Jahr.dat</t>
+  </si>
+  <si>
+    <t>TRY2015_515220074856_Jahr.dat</t>
+  </si>
+  <si>
+    <t>TRY2015_522733105384_Jahr.dat</t>
+  </si>
+  <si>
+    <t>TRY2015_507755060854_Jahr.dat</t>
   </si>
 </sst>
 </file>
@@ -164,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -172,6 +145,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -474,13 +449,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="39" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -503,8 +481,8 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>6</v>
+      <c r="A2" s="4">
+        <v>44137</v>
       </c>
       <c r="B2">
         <v>51.057549599999987</v>
@@ -513,7 +491,7 @@
         <v>13.717064799999999</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E2">
         <v>51.06157970077107</v>
@@ -523,8 +501,8 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>8</v>
+      <c r="A3" s="3">
+        <v>50667</v>
       </c>
       <c r="B3">
         <v>51.039134900000001</v>
@@ -533,7 +511,7 @@
         <v>13.737674800000001</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E3">
         <v>51.042046308508112</v>
@@ -543,8 +521,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>10</v>
+      <c r="A4" s="3">
+        <v>52064</v>
       </c>
       <c r="B4">
         <v>51.065908100000001</v>
@@ -553,7 +531,7 @@
         <v>13.736152499999999</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E4">
         <v>51.070407627228121</v>
@@ -563,8 +541,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>12</v>
+      <c r="A5" s="3">
+        <v>34117</v>
       </c>
       <c r="B5">
         <v>51.087188400000002</v>
@@ -573,7 +551,7 @@
         <v>13.8028038</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5">
         <v>51.086627310398377</v>
@@ -583,8 +561,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>14</v>
+      <c r="A6" s="3">
+        <v>10115</v>
       </c>
       <c r="B6">
         <v>51.144323900000003</v>
@@ -593,7 +571,7 @@
         <v>13.799705700000001</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E6">
         <v>51.142883954834232</v>
@@ -603,8 +581,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>16</v>
+      <c r="A7" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="B7">
         <v>51.1173979</v>
@@ -613,7 +591,7 @@
         <v>13.728314900000001</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E7">
         <v>51.117361114561781</v>
@@ -623,8 +601,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>18</v>
+      <c r="A8" s="3">
+        <v>80331</v>
       </c>
       <c r="B8">
         <v>51.077936600000001</v>
@@ -633,7 +611,7 @@
         <v>13.722437899999999</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E8">
         <v>51.080173609669671</v>
@@ -643,8 +621,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>20</v>
+      <c r="A9" s="3">
+        <v>20354</v>
       </c>
       <c r="B9">
         <v>51.0943744</v>
@@ -653,7 +631,7 @@
         <v>13.7205411</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="E9">
         <v>51.098767414925582</v>
@@ -663,8 +641,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>22</v>
+      <c r="A10" s="3">
+        <v>79100</v>
       </c>
       <c r="B10">
         <v>51.074711899999997</v>
@@ -673,7 +651,7 @@
         <v>13.684631400000001</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E10">
         <v>51.071809179759093</v>
@@ -683,8 +661,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>24</v>
+      <c r="A11" s="3">
+        <v>38100</v>
       </c>
       <c r="B11">
         <v>51.085543999999999</v>
@@ -693,7 +671,7 @@
         <v>13.6276849</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E11">
         <v>51.082949411534422</v>
@@ -702,47 +680,8 @@
         <v>13.629674415765569</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12">
-        <v>51.057549599999987</v>
-      </c>
-      <c r="C12">
-        <v>13.717064799999999</v>
-      </c>
-      <c r="D12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12">
-        <v>51.06157970077107</v>
-      </c>
-      <c r="F12">
-        <v>13.71674948054328</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13">
-        <v>51.039134900000001</v>
-      </c>
-      <c r="C13">
-        <v>13.737674800000001</v>
-      </c>
-      <c r="D13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13">
-        <v>51.042046308508112</v>
-      </c>
-      <c r="F13">
-        <v>13.74475915535144</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>